<commit_message>
Add domestic EPU calculation with updated foreign country data
- Downloaded All_Country_Data.xlsx from policyuncertainty.com (data through Oct 2025)
- Created dataset_est_domestic_updated.xlsx with mapped country columns
- Updated calculate_epu_complete.py to use new methodology:
  - Estimates regression using 487 months of historical Ireland EPU data
  - R² = 0.6358 for Ireland EPU ~ weighted_PCA + 3 lags
  - Applies coefficients to calculate domestic EPU for scraped months
  - Domestic EPU = Main EPU - Foreign-driven component (scaled)

Domestic EPU now calculated for Jun-Oct 2025:
- Jun 2025: Main=433.10, Domestic=57.37
- Jul 2025: Main=452.45, Domestic=94.69
- Aug 2025: Main=239.67, Domestic=-54.64
- Sep 2025: Main=262.52, Domestic=-16.55
- Oct 2025: Main=294.34, Domestic=35.13

Nov 2025 - Jan 2026 domestic EPU pending updated foreign data.

https://claude.ai/code/session_01DCSPnRckBQ9nL9EWNUMffT
</commit_message>
<xml_diff>
--- a/out_fast_epu_scrape/ireland_epu_jun2025_jan2026.xlsx
+++ b/out_fast_epu_scrape/ireland_epu_jun2025_jan2026.xlsx
@@ -444,7 +444,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>2026-02-04 17:49:30</t>
+          <t>2026-02-04 18:00:32</t>
         </is>
       </c>
     </row>
@@ -585,7 +585,9 @@
       <c r="E2" t="n">
         <v>433.0988321194267</v>
       </c>
-      <c r="F2" t="inlineStr"/>
+      <c r="F2" t="n">
+        <v>57.36575675314314</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -605,7 +607,9 @@
       <c r="E3" t="n">
         <v>452.4533845229234</v>
       </c>
-      <c r="F3" t="inlineStr"/>
+      <c r="F3" t="n">
+        <v>94.69138610935934</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -625,7 +629,9 @@
       <c r="E4" t="n">
         <v>239.6704198273313</v>
       </c>
-      <c r="F4" t="inlineStr"/>
+      <c r="F4" t="n">
+        <v>-54.63860549041632</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -645,7 +651,9 @@
       <c r="E5" t="n">
         <v>262.5229241438968</v>
       </c>
-      <c r="F5" t="inlineStr"/>
+      <c r="F5" t="n">
+        <v>-16.55135733179955</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -665,7 +673,9 @@
       <c r="E6" t="n">
         <v>294.3449057905248</v>
       </c>
-      <c r="F6" t="inlineStr"/>
+      <c r="F6" t="n">
+        <v>35.12546384883223</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -772,7 +782,9 @@
       <c r="B2" t="n">
         <v>433.0988321194267</v>
       </c>
-      <c r="C2" t="inlineStr"/>
+      <c r="C2" t="n">
+        <v>57.36575675314314</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -783,7 +795,9 @@
       <c r="B3" t="n">
         <v>318.2155761647172</v>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>7.833807762381156</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -794,7 +808,9 @@
       <c r="B4" t="n">
         <v>257.6258096786369</v>
       </c>
-      <c r="C4" t="inlineStr"/>
+      <c r="C4" t="n">
+        <v>35.12546384883223</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">

</xml_diff>